<commit_message>
REAIS 3.3 --> UNI + figuras + apresentações
</commit_message>
<xml_diff>
--- a/Apresentacoes/PARAMETROSLIVRES_1.xlsx
+++ b/Apresentacoes/PARAMETROSLIVRES_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14460" windowHeight="7905"/>
+    <workbookView windowWidth="19485" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
   <si>
     <t>GRIEWANGK</t>
   </si>
@@ -75,16 +75,31 @@
   <si>
     <t>NOVO DEPOIS DE ARRUMAR</t>
   </si>
+  <si>
+    <t>std | por</t>
+  </si>
+  <si>
+    <t>GEOreal2_P_VO_UNI</t>
+  </si>
+  <si>
+    <t>GEOreal2_N_VO_UNI</t>
+  </si>
+  <si>
+    <t>GEOreal2_P_DS_UNI</t>
+  </si>
+  <si>
+    <t>GEOreal2_N_DS_UNI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -112,6 +127,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -127,7 +156,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,21 +210,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,29 +254,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -200,54 +261,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,13 +271,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,97 +445,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,67 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,15 +631,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -628,17 +646,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,26 +675,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -695,6 +696,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -706,142 +733,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -851,7 +878,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -903,6 +930,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,6 +945,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -933,7 +975,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1261,16 +1312,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:AA34"/>
+  <dimension ref="B1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O22" workbookViewId="0">
-      <selection activeCell="Z47" sqref="Z47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.75" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15"/>
@@ -1280,37 +1331,37 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="20"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="20"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="20"/>
+      <c r="N2" s="25"/>
       <c r="O2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="20"/>
+      <c r="R2" s="25"/>
       <c r="S2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="20"/>
+      <c r="V2" s="25"/>
       <c r="W2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="20"/>
+      <c r="Z2" s="25"/>
     </row>
     <row r="3" ht="15" spans="3:26">
       <c r="C3" s="3" t="s">
@@ -1322,7 +1373,7 @@
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1334,7 +1385,7 @@
       <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -1346,7 +1397,7 @@
       <c r="M3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -1358,7 +1409,7 @@
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S3" s="3" t="s">
@@ -1370,7 +1421,7 @@
       <c r="U3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="W3" s="3" t="s">
@@ -1382,7 +1433,7 @@
       <c r="Y3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="21" t="s">
+      <c r="Z3" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1394,42 +1445,42 @@
       <c r="E4">
         <v>0.8</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="27">
         <v>1.5</v>
       </c>
       <c r="G4" s="6"/>
       <c r="I4">
         <v>1.2</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="27">
         <v>1.5</v>
       </c>
       <c r="K4" s="6"/>
       <c r="M4">
         <v>2.4</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="27">
         <v>6.5</v>
       </c>
       <c r="O4" s="6"/>
       <c r="Q4">
         <v>0.6</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="27">
         <v>8</v>
       </c>
       <c r="S4" s="6"/>
       <c r="U4">
         <v>0.8</v>
       </c>
-      <c r="V4" s="22">
+      <c r="V4" s="27">
         <v>1</v>
       </c>
       <c r="W4" s="6"/>
       <c r="Y4">
         <v>2</v>
       </c>
-      <c r="Z4" s="22">
+      <c r="Z4" s="27">
         <v>6</v>
       </c>
     </row>
@@ -1441,42 +1492,42 @@
       <c r="E5">
         <v>0.5</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="27">
         <v>4.5</v>
       </c>
       <c r="G5" s="6"/>
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="27">
         <v>5</v>
       </c>
       <c r="K5" s="6"/>
       <c r="M5">
         <v>0.5</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="27">
         <v>4.5</v>
       </c>
       <c r="O5" s="6"/>
       <c r="Q5">
         <v>7.5</v>
       </c>
-      <c r="R5" s="22">
+      <c r="R5" s="27">
         <v>3</v>
       </c>
       <c r="S5" s="6"/>
       <c r="U5">
         <v>1</v>
       </c>
-      <c r="V5" s="22">
+      <c r="V5" s="27">
         <v>5</v>
       </c>
       <c r="W5" s="6"/>
       <c r="Y5">
         <v>3</v>
       </c>
-      <c r="Z5" s="22">
+      <c r="Z5" s="27">
         <v>4</v>
       </c>
     </row>
@@ -1488,42 +1539,42 @@
       <c r="E6">
         <v>1.8</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="27">
         <v>1.5</v>
       </c>
       <c r="G6" s="6"/>
       <c r="I6">
         <v>0.4</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="27">
         <v>6</v>
       </c>
       <c r="K6" s="6"/>
       <c r="M6">
         <v>0.2</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="27">
         <v>5.5</v>
       </c>
       <c r="O6" s="6"/>
       <c r="Q6">
         <v>1.8</v>
       </c>
-      <c r="R6" s="22">
+      <c r="R6" s="27">
         <v>2</v>
       </c>
       <c r="S6" s="6"/>
       <c r="U6">
         <v>0.4</v>
       </c>
-      <c r="V6" s="22">
+      <c r="V6" s="27">
         <v>6.5</v>
       </c>
       <c r="W6" s="6"/>
       <c r="Y6">
         <v>0.2</v>
       </c>
-      <c r="Z6" s="22">
+      <c r="Z6" s="27">
         <v>2</v>
       </c>
     </row>
@@ -1540,7 +1591,7 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="27">
         <v>3</v>
       </c>
       <c r="G7" s="6">
@@ -1552,7 +1603,7 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="27">
         <v>5</v>
       </c>
       <c r="K7" s="6">
@@ -1564,7 +1615,7 @@
       <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="27">
         <v>5</v>
       </c>
       <c r="O7" s="6">
@@ -1576,7 +1627,7 @@
       <c r="Q7">
         <v>4</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="27">
         <v>5</v>
       </c>
       <c r="S7" s="6">
@@ -1588,7 +1639,7 @@
       <c r="U7">
         <v>1</v>
       </c>
-      <c r="V7" s="22">
+      <c r="V7" s="27">
         <v>5</v>
       </c>
       <c r="W7" s="6">
@@ -1600,7 +1651,7 @@
       <c r="Y7">
         <v>1</v>
       </c>
-      <c r="Z7" s="22">
+      <c r="Z7" s="27">
         <v>3.5</v>
       </c>
     </row>
@@ -1617,7 +1668,7 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="27">
         <v>2.5</v>
       </c>
       <c r="G8" s="6">
@@ -1629,7 +1680,7 @@
       <c r="I8">
         <v>10</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="27">
         <v>5</v>
       </c>
       <c r="K8" s="6">
@@ -1641,7 +1692,7 @@
       <c r="M8">
         <v>0.3</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="27">
         <v>5</v>
       </c>
       <c r="O8" s="6">
@@ -1653,7 +1704,7 @@
       <c r="Q8">
         <v>10</v>
       </c>
-      <c r="R8" s="22">
+      <c r="R8" s="27">
         <v>3</v>
       </c>
       <c r="S8" s="6">
@@ -1665,7 +1716,7 @@
       <c r="U8">
         <v>5</v>
       </c>
-      <c r="V8" s="22">
+      <c r="V8" s="27">
         <v>5</v>
       </c>
       <c r="W8" s="6">
@@ -1677,7 +1728,7 @@
       <c r="Y8">
         <v>10</v>
       </c>
-      <c r="Z8" s="22">
+      <c r="Z8" s="27">
         <v>4</v>
       </c>
     </row>
@@ -1694,7 +1745,7 @@
       <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="27">
         <v>3</v>
       </c>
       <c r="G9" s="6">
@@ -1706,7 +1757,7 @@
       <c r="I9">
         <v>4</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="27">
         <v>5</v>
       </c>
       <c r="K9" s="6">
@@ -1718,7 +1769,7 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="27">
         <v>4.5</v>
       </c>
       <c r="O9" s="6">
@@ -1730,7 +1781,7 @@
       <c r="Q9">
         <v>4</v>
       </c>
-      <c r="R9" s="22">
+      <c r="R9" s="27">
         <v>3</v>
       </c>
       <c r="S9" s="6">
@@ -1742,7 +1793,7 @@
       <c r="U9">
         <v>4</v>
       </c>
-      <c r="V9" s="22">
+      <c r="V9" s="27">
         <v>5</v>
       </c>
       <c r="W9" s="6">
@@ -1754,7 +1805,7 @@
       <c r="Y9">
         <v>2</v>
       </c>
-      <c r="Z9" s="22">
+      <c r="Z9" s="27">
         <v>3.5</v>
       </c>
     </row>
@@ -1771,7 +1822,7 @@
       <c r="E10">
         <v>5</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="27">
         <v>4</v>
       </c>
       <c r="G10" s="6">
@@ -1783,7 +1834,7 @@
       <c r="I10">
         <v>5</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="27">
         <v>4.5</v>
       </c>
       <c r="K10" s="6">
@@ -1795,7 +1846,7 @@
       <c r="M10">
         <v>5</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="27">
         <v>4</v>
       </c>
       <c r="O10" s="6">
@@ -1807,7 +1858,7 @@
       <c r="Q10">
         <v>5</v>
       </c>
-      <c r="R10" s="22">
+      <c r="R10" s="27">
         <v>5</v>
       </c>
       <c r="S10" s="6">
@@ -1819,7 +1870,7 @@
       <c r="U10">
         <v>1</v>
       </c>
-      <c r="V10" s="22">
+      <c r="V10" s="27">
         <v>5</v>
       </c>
       <c r="W10" s="6">
@@ -1831,7 +1882,7 @@
       <c r="Y10">
         <v>1</v>
       </c>
-      <c r="Z10" s="22">
+      <c r="Z10" s="27">
         <v>3</v>
       </c>
     </row>
@@ -1848,7 +1899,7 @@
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="27">
         <v>2.5</v>
       </c>
       <c r="G11" s="6">
@@ -1860,7 +1911,7 @@
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="27">
         <v>5</v>
       </c>
       <c r="K11" s="6">
@@ -1872,7 +1923,7 @@
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="27">
         <v>5</v>
       </c>
       <c r="O11" s="6">
@@ -1884,7 +1935,7 @@
       <c r="Q11">
         <v>50</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="27">
         <v>4.5</v>
       </c>
       <c r="S11" s="6">
@@ -1896,7 +1947,7 @@
       <c r="U11">
         <v>10</v>
       </c>
-      <c r="V11" s="22">
+      <c r="V11" s="27">
         <v>5</v>
       </c>
       <c r="W11" s="6">
@@ -1908,7 +1959,7 @@
       <c r="Y11">
         <v>10</v>
       </c>
-      <c r="Z11" s="22">
+      <c r="Z11" s="27">
         <v>3.5</v>
       </c>
     </row>
@@ -1925,7 +1976,7 @@
       <c r="E12" s="10">
         <v>10</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="28">
         <v>4.5</v>
       </c>
       <c r="G12" s="9">
@@ -1937,7 +1988,7 @@
       <c r="I12" s="10">
         <v>10</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="28">
         <v>5</v>
       </c>
       <c r="K12" s="9">
@@ -1949,7 +2000,7 @@
       <c r="M12" s="10">
         <v>1</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="28">
         <v>4</v>
       </c>
       <c r="O12" s="9">
@@ -1961,7 +2012,7 @@
       <c r="Q12" s="10">
         <v>10</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="28">
         <v>2</v>
       </c>
       <c r="S12" s="9">
@@ -1973,7 +2024,7 @@
       <c r="U12" s="10">
         <v>10</v>
       </c>
-      <c r="V12" s="23">
+      <c r="V12" s="28">
         <v>4.5</v>
       </c>
       <c r="W12" s="9">
@@ -1985,7 +2036,7 @@
       <c r="Y12" s="10">
         <v>10</v>
       </c>
-      <c r="Z12" s="23">
+      <c r="Z12" s="28">
         <v>3</v>
       </c>
     </row>
@@ -1994,29 +2045,29 @@
       <c r="D18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="36"/>
     </row>
     <row r="19" ht="15" spans="4:14">
       <c r="D19" s="12"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="37"/>
     </row>
     <row r="23" ht="15"/>
     <row r="24" ht="15" spans="3:26">
@@ -2025,39 +2076,39 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="20"/>
+      <c r="F24" s="25"/>
       <c r="G24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="20"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="20"/>
+      <c r="N24" s="25"/>
       <c r="O24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="20"/>
+      <c r="R24" s="25"/>
       <c r="S24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="20"/>
+      <c r="V24" s="25"/>
       <c r="W24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-      <c r="Z24" s="20"/>
+      <c r="Z24" s="25"/>
     </row>
-    <row r="25" spans="3:26">
+    <row r="25" ht="15" spans="3:26">
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
@@ -2067,7 +2118,7 @@
       <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="26" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -2077,9 +2128,9 @@
         <v>7</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="26" t="s">
         <v>9</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -2091,7 +2142,7 @@
       <c r="M25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N25" s="21" t="s">
+      <c r="N25" s="26" t="s">
         <v>9</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -2103,7 +2154,7 @@
       <c r="Q25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R25" s="21" t="s">
+      <c r="R25" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -2115,7 +2166,7 @@
       <c r="U25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V25" s="21" t="s">
+      <c r="V25" s="26" t="s">
         <v>9</v>
       </c>
       <c r="W25" s="3" t="s">
@@ -2127,7 +2178,7 @@
       <c r="Y25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Z25" s="21" t="s">
+      <c r="Z25" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2140,7 +2191,7 @@
       <c r="E26" s="15">
         <v>1</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="31">
         <v>1.5</v>
       </c>
       <c r="G26" s="14"/>
@@ -2148,7 +2199,7 @@
       <c r="I26" s="15">
         <v>1.8</v>
       </c>
-      <c r="J26" s="26">
+      <c r="J26" s="31">
         <v>2</v>
       </c>
       <c r="K26" s="14"/>
@@ -2156,7 +2207,7 @@
       <c r="M26" s="15">
         <v>2.2</v>
       </c>
-      <c r="N26" s="26">
+      <c r="N26" s="31">
         <v>6</v>
       </c>
       <c r="O26" s="14"/>
@@ -2164,7 +2215,7 @@
       <c r="Q26" s="15">
         <v>1.8</v>
       </c>
-      <c r="R26" s="26">
+      <c r="R26" s="31">
         <v>6</v>
       </c>
       <c r="S26" s="14"/>
@@ -2172,7 +2223,7 @@
       <c r="U26" s="15">
         <v>0.8</v>
       </c>
-      <c r="V26" s="26">
+      <c r="V26" s="31">
         <v>1</v>
       </c>
       <c r="W26" s="14"/>
@@ -2180,7 +2231,7 @@
       <c r="Y26" s="15">
         <v>2</v>
       </c>
-      <c r="Z26" s="26">
+      <c r="Z26" s="31">
         <v>5</v>
       </c>
       <c r="AA26" s="15"/>
@@ -2194,7 +2245,7 @@
       <c r="E27" s="15">
         <v>0.5</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="31">
         <v>6</v>
       </c>
       <c r="G27" s="14"/>
@@ -2202,7 +2253,7 @@
       <c r="I27" s="15">
         <v>3</v>
       </c>
-      <c r="J27" s="26">
+      <c r="J27" s="31">
         <v>5</v>
       </c>
       <c r="K27" s="14"/>
@@ -2210,7 +2261,7 @@
       <c r="M27" s="15">
         <v>0.5</v>
       </c>
-      <c r="N27" s="26">
+      <c r="N27" s="31">
         <v>6</v>
       </c>
       <c r="O27" s="14"/>
@@ -2218,7 +2269,7 @@
       <c r="Q27" s="15">
         <v>8</v>
       </c>
-      <c r="R27" s="26">
+      <c r="R27" s="31">
         <v>2.5</v>
       </c>
       <c r="S27" s="14"/>
@@ -2226,7 +2277,7 @@
       <c r="U27" s="15">
         <v>1</v>
       </c>
-      <c r="V27" s="26">
+      <c r="V27" s="31">
         <v>5</v>
       </c>
       <c r="W27" s="14"/>
@@ -2234,7 +2285,7 @@
       <c r="Y27" s="15">
         <v>1.5</v>
       </c>
-      <c r="Z27" s="26">
+      <c r="Z27" s="31">
         <v>1.5</v>
       </c>
       <c r="AA27" s="15"/>
@@ -2248,7 +2299,7 @@
       <c r="E28" s="15">
         <v>2</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="31">
         <v>1.5</v>
       </c>
       <c r="G28" s="14"/>
@@ -2256,7 +2307,7 @@
       <c r="I28" s="15">
         <v>0.4</v>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="31">
         <v>6</v>
       </c>
       <c r="K28" s="14"/>
@@ -2264,7 +2315,7 @@
       <c r="M28" s="15">
         <v>0.2</v>
       </c>
-      <c r="N28" s="26">
+      <c r="N28" s="31">
         <v>5</v>
       </c>
       <c r="O28" s="14"/>
@@ -2272,7 +2323,7 @@
       <c r="Q28" s="15">
         <v>1.4</v>
       </c>
-      <c r="R28" s="26">
+      <c r="R28" s="31">
         <v>1.5</v>
       </c>
       <c r="S28" s="14"/>
@@ -2280,7 +2331,7 @@
       <c r="U28" s="15">
         <v>0.6</v>
       </c>
-      <c r="V28" s="26">
+      <c r="V28" s="31">
         <v>6</v>
       </c>
       <c r="W28" s="14"/>
@@ -2288,7 +2339,7 @@
       <c r="Y28" s="15">
         <v>0.2</v>
       </c>
-      <c r="Z28" s="26">
+      <c r="Z28" s="31">
         <v>2</v>
       </c>
       <c r="AA28" s="15"/>
@@ -2306,7 +2357,7 @@
       <c r="E29" s="15">
         <v>1</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="31">
         <v>2.5</v>
       </c>
       <c r="G29" s="14">
@@ -2318,7 +2369,7 @@
       <c r="I29" s="15">
         <v>1</v>
       </c>
-      <c r="J29" s="26">
+      <c r="J29" s="31">
         <v>4.5</v>
       </c>
       <c r="K29" s="14">
@@ -2330,7 +2381,7 @@
       <c r="M29" s="15">
         <v>1</v>
       </c>
-      <c r="N29" s="26">
+      <c r="N29" s="31">
         <v>5</v>
       </c>
       <c r="O29" s="14">
@@ -2342,7 +2393,7 @@
       <c r="Q29" s="15">
         <v>8</v>
       </c>
-      <c r="R29" s="26">
+      <c r="R29" s="31">
         <v>4</v>
       </c>
       <c r="S29" s="14">
@@ -2354,7 +2405,7 @@
       <c r="U29" s="15">
         <v>1</v>
       </c>
-      <c r="V29" s="26">
+      <c r="V29" s="31">
         <v>5</v>
       </c>
       <c r="W29" s="14">
@@ -2366,85 +2417,85 @@
       <c r="Y29" s="15">
         <v>2</v>
       </c>
-      <c r="Z29" s="26">
+      <c r="Z29" s="31">
         <v>4</v>
       </c>
       <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="2:27">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="15">
-        <v>12</v>
-      </c>
-      <c r="D30" s="15">
-        <v>1</v>
-      </c>
-      <c r="E30" s="15">
-        <v>10</v>
-      </c>
-      <c r="F30" s="15">
-        <v>3</v>
-      </c>
-      <c r="G30" s="14">
-        <v>12</v>
-      </c>
-      <c r="H30" s="15">
-        <v>2</v>
-      </c>
-      <c r="I30" s="15">
-        <v>10</v>
-      </c>
-      <c r="J30" s="26">
-        <v>5</v>
-      </c>
-      <c r="K30" s="14">
-        <v>4</v>
-      </c>
-      <c r="L30" s="15">
-        <v>1</v>
-      </c>
-      <c r="M30" s="15">
+      <c r="C30" s="18">
+        <v>12</v>
+      </c>
+      <c r="D30" s="18">
+        <v>1</v>
+      </c>
+      <c r="E30" s="18">
+        <v>1</v>
+      </c>
+      <c r="F30" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="G30" s="32">
+        <v>12</v>
+      </c>
+      <c r="H30" s="18">
+        <v>2</v>
+      </c>
+      <c r="I30" s="18">
+        <v>10</v>
+      </c>
+      <c r="J30" s="35">
+        <v>5</v>
+      </c>
+      <c r="K30" s="32">
+        <v>4</v>
+      </c>
+      <c r="L30" s="18">
+        <v>1</v>
+      </c>
+      <c r="M30" s="18">
         <v>0.1</v>
       </c>
-      <c r="N30" s="26">
-        <v>4</v>
-      </c>
-      <c r="O30" s="14">
-        <v>12</v>
-      </c>
-      <c r="P30" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q30" s="15">
+      <c r="N30" s="35">
+        <v>4</v>
+      </c>
+      <c r="O30" s="32">
+        <v>12</v>
+      </c>
+      <c r="P30" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="18">
         <v>50</v>
       </c>
-      <c r="R30" s="26">
-        <v>5</v>
-      </c>
-      <c r="S30" s="14">
-        <v>12</v>
-      </c>
-      <c r="T30" s="15">
-        <v>2</v>
-      </c>
-      <c r="U30" s="15">
-        <v>10</v>
-      </c>
-      <c r="V30" s="26">
-        <v>5</v>
-      </c>
-      <c r="W30" s="14">
-        <v>12</v>
-      </c>
-      <c r="X30" s="15">
-        <v>1</v>
-      </c>
-      <c r="Y30" s="15">
+      <c r="R30" s="35">
+        <v>5</v>
+      </c>
+      <c r="S30" s="32">
+        <v>12</v>
+      </c>
+      <c r="T30" s="18">
+        <v>2</v>
+      </c>
+      <c r="U30" s="18">
+        <v>10</v>
+      </c>
+      <c r="V30" s="35">
+        <v>5</v>
+      </c>
+      <c r="W30" s="32">
+        <v>12</v>
+      </c>
+      <c r="X30" s="18">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="18">
         <v>50</v>
       </c>
-      <c r="Z30" s="26">
+      <c r="Z30" s="35">
         <v>3.5</v>
       </c>
       <c r="AA30" s="15"/>
@@ -2462,7 +2513,7 @@
       <c r="E31" s="15">
         <v>2</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="31">
         <v>2.5</v>
       </c>
       <c r="G31" s="14">
@@ -2474,7 +2525,7 @@
       <c r="I31" s="15">
         <v>1</v>
       </c>
-      <c r="J31" s="26">
+      <c r="J31" s="31">
         <v>5</v>
       </c>
       <c r="K31" s="14">
@@ -2486,7 +2537,7 @@
       <c r="M31" s="15">
         <v>0.5</v>
       </c>
-      <c r="N31" s="26">
+      <c r="N31" s="31">
         <v>5</v>
       </c>
       <c r="O31" s="14">
@@ -2498,7 +2549,7 @@
       <c r="Q31" s="15">
         <v>2</v>
       </c>
-      <c r="R31" s="26">
+      <c r="R31" s="31">
         <v>4</v>
       </c>
       <c r="S31" s="14">
@@ -2510,7 +2561,7 @@
       <c r="U31" s="15">
         <v>2</v>
       </c>
-      <c r="V31" s="26">
+      <c r="V31" s="31">
         <v>4.5</v>
       </c>
       <c r="W31" s="14">
@@ -2522,7 +2573,7 @@
       <c r="Y31" s="15">
         <v>2</v>
       </c>
-      <c r="Z31" s="26">
+      <c r="Z31" s="31">
         <v>2.5</v>
       </c>
       <c r="AA31" s="15"/>
@@ -2540,7 +2591,7 @@
       <c r="E32" s="15">
         <v>5</v>
       </c>
-      <c r="F32" s="26">
+      <c r="F32" s="31">
         <v>5</v>
       </c>
       <c r="G32" s="14">
@@ -2552,7 +2603,7 @@
       <c r="I32" s="15">
         <v>5</v>
       </c>
-      <c r="J32" s="26">
+      <c r="J32" s="31">
         <v>4.5</v>
       </c>
       <c r="K32" s="14">
@@ -2564,7 +2615,7 @@
       <c r="M32" s="15">
         <v>5</v>
       </c>
-      <c r="N32" s="26">
+      <c r="N32" s="31">
         <v>5</v>
       </c>
       <c r="O32" s="14">
@@ -2576,7 +2627,7 @@
       <c r="Q32" s="15">
         <v>5</v>
       </c>
-      <c r="R32" s="26">
+      <c r="R32" s="31">
         <v>5</v>
       </c>
       <c r="S32" s="14">
@@ -2588,7 +2639,7 @@
       <c r="U32" s="15">
         <v>1</v>
       </c>
-      <c r="V32" s="26">
+      <c r="V32" s="31">
         <v>5</v>
       </c>
       <c r="W32" s="14">
@@ -2600,7 +2651,7 @@
       <c r="Y32" s="15">
         <v>1</v>
       </c>
-      <c r="Z32" s="26">
+      <c r="Z32" s="31">
         <v>5</v>
       </c>
       <c r="AA32" s="15"/>
@@ -2618,7 +2669,7 @@
       <c r="E33" s="15">
         <v>5</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="31">
         <v>3</v>
       </c>
       <c r="G33" s="14">
@@ -2630,7 +2681,7 @@
       <c r="I33" s="15">
         <v>10</v>
       </c>
-      <c r="J33" s="26">
+      <c r="J33" s="31">
         <v>4.5</v>
       </c>
       <c r="K33" s="14">
@@ -2642,7 +2693,7 @@
       <c r="M33" s="15">
         <v>0.1</v>
       </c>
-      <c r="N33" s="26">
+      <c r="N33" s="31">
         <v>5</v>
       </c>
       <c r="O33" s="14">
@@ -2654,7 +2705,7 @@
       <c r="Q33" s="15">
         <v>50</v>
       </c>
-      <c r="R33" s="26">
+      <c r="R33" s="31">
         <v>4.5</v>
       </c>
       <c r="S33" s="14">
@@ -2666,7 +2717,7 @@
       <c r="U33" s="15">
         <v>5</v>
       </c>
-      <c r="V33" s="26">
+      <c r="V33" s="31">
         <v>5</v>
       </c>
       <c r="W33" s="14">
@@ -2678,88 +2729,396 @@
       <c r="Y33" s="15">
         <v>50</v>
       </c>
-      <c r="Z33" s="26">
+      <c r="Z33" s="31">
         <v>3</v>
       </c>
       <c r="AA33" s="15"/>
     </row>
-    <row r="34" spans="2:27">
-      <c r="B34" s="17" t="s">
+    <row r="34" ht="15" spans="2:27">
+      <c r="B34" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="18">
-        <v>4</v>
-      </c>
-      <c r="D34" s="19">
-        <v>10</v>
-      </c>
-      <c r="E34" s="19">
-        <v>5</v>
-      </c>
-      <c r="F34" s="27">
-        <v>4</v>
-      </c>
-      <c r="G34" s="18">
+      <c r="C34" s="20">
+        <v>4</v>
+      </c>
+      <c r="D34" s="21">
+        <v>10</v>
+      </c>
+      <c r="E34" s="21">
+        <v>5</v>
+      </c>
+      <c r="F34" s="33">
+        <v>4</v>
+      </c>
+      <c r="G34" s="20">
         <v>16</v>
       </c>
-      <c r="H34" s="19">
-        <v>10</v>
-      </c>
-      <c r="I34" s="19">
-        <v>10</v>
-      </c>
-      <c r="J34" s="27">
-        <v>5</v>
-      </c>
-      <c r="K34" s="18">
+      <c r="H34" s="21">
+        <v>10</v>
+      </c>
+      <c r="I34" s="21">
+        <v>10</v>
+      </c>
+      <c r="J34" s="33">
+        <v>5</v>
+      </c>
+      <c r="K34" s="20">
         <v>8</v>
       </c>
-      <c r="L34" s="19">
-        <v>2</v>
-      </c>
-      <c r="M34" s="19">
-        <v>1</v>
-      </c>
-      <c r="N34" s="27">
-        <v>5</v>
-      </c>
-      <c r="O34" s="18">
-        <v>4</v>
-      </c>
-      <c r="P34" s="19">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="19">
-        <v>10</v>
-      </c>
-      <c r="R34" s="27">
+      <c r="L34" s="21">
+        <v>2</v>
+      </c>
+      <c r="M34" s="21">
+        <v>1</v>
+      </c>
+      <c r="N34" s="33">
+        <v>5</v>
+      </c>
+      <c r="O34" s="20">
+        <v>4</v>
+      </c>
+      <c r="P34" s="21">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>10</v>
+      </c>
+      <c r="R34" s="33">
         <v>0.5</v>
       </c>
-      <c r="S34" s="18">
+      <c r="S34" s="20">
         <v>16</v>
       </c>
-      <c r="T34" s="19">
-        <v>10</v>
-      </c>
-      <c r="U34" s="19">
-        <v>5</v>
-      </c>
-      <c r="V34" s="27">
-        <v>5</v>
-      </c>
-      <c r="W34" s="18">
+      <c r="T34" s="21">
+        <v>10</v>
+      </c>
+      <c r="U34" s="21">
+        <v>5</v>
+      </c>
+      <c r="V34" s="33">
+        <v>5</v>
+      </c>
+      <c r="W34" s="20">
         <v>16</v>
       </c>
-      <c r="X34" s="19">
-        <v>2</v>
-      </c>
-      <c r="Y34" s="19">
-        <v>5</v>
-      </c>
-      <c r="Z34" s="27">
+      <c r="X34" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y34" s="21">
+        <v>5</v>
+      </c>
+      <c r="Z34" s="33">
         <v>2.5</v>
       </c>
       <c r="AA34" s="15"/>
+    </row>
+    <row r="35" spans="2:26">
+      <c r="B35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="23">
+        <v>12</v>
+      </c>
+      <c r="D35" s="24">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24">
+        <v>1</v>
+      </c>
+      <c r="F35" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="G35" s="23">
+        <v>12</v>
+      </c>
+      <c r="H35" s="24">
+        <v>2</v>
+      </c>
+      <c r="I35" s="24">
+        <v>10</v>
+      </c>
+      <c r="J35" s="34">
+        <v>5</v>
+      </c>
+      <c r="K35" s="23">
+        <v>4</v>
+      </c>
+      <c r="L35" s="24">
+        <v>1</v>
+      </c>
+      <c r="M35" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="N35" s="34">
+        <v>4</v>
+      </c>
+      <c r="O35" s="23">
+        <v>12</v>
+      </c>
+      <c r="P35" s="24">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="24">
+        <v>50</v>
+      </c>
+      <c r="R35" s="34">
+        <v>5</v>
+      </c>
+      <c r="S35" s="23">
+        <v>12</v>
+      </c>
+      <c r="T35" s="24">
+        <v>2</v>
+      </c>
+      <c r="U35" s="24">
+        <v>10</v>
+      </c>
+      <c r="V35" s="34">
+        <v>5</v>
+      </c>
+      <c r="W35" s="23">
+        <v>12</v>
+      </c>
+      <c r="X35" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="24">
+        <v>50</v>
+      </c>
+      <c r="Z35" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:26">
+      <c r="B36" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="14">
+        <v>4</v>
+      </c>
+      <c r="D36" s="15">
+        <v>2</v>
+      </c>
+      <c r="E36" s="15">
+        <v>2</v>
+      </c>
+      <c r="F36" s="31">
+        <v>2.5</v>
+      </c>
+      <c r="G36" s="14">
+        <v>12</v>
+      </c>
+      <c r="H36" s="15">
+        <v>2</v>
+      </c>
+      <c r="I36" s="15">
+        <v>2</v>
+      </c>
+      <c r="J36" s="31">
+        <v>5</v>
+      </c>
+      <c r="K36" s="14">
+        <v>4</v>
+      </c>
+      <c r="L36" s="15">
+        <v>2</v>
+      </c>
+      <c r="M36" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="N36" s="31">
+        <v>5</v>
+      </c>
+      <c r="O36" s="14">
+        <v>12</v>
+      </c>
+      <c r="P36" s="15">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="15">
+        <v>2</v>
+      </c>
+      <c r="R36" s="31">
+        <v>4</v>
+      </c>
+      <c r="S36" s="14">
+        <v>12</v>
+      </c>
+      <c r="T36" s="15">
+        <v>2</v>
+      </c>
+      <c r="U36" s="15">
+        <v>2</v>
+      </c>
+      <c r="V36" s="31">
+        <v>5</v>
+      </c>
+      <c r="W36" s="14">
+        <v>12</v>
+      </c>
+      <c r="X36" s="15">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="15">
+        <v>2</v>
+      </c>
+      <c r="Z36" s="31">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:26">
+      <c r="B37" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="14">
+        <v>4</v>
+      </c>
+      <c r="D37" s="15">
+        <v>10</v>
+      </c>
+      <c r="E37" s="15">
+        <v>1</v>
+      </c>
+      <c r="F37" s="31">
+        <v>4</v>
+      </c>
+      <c r="G37" s="14">
+        <v>12</v>
+      </c>
+      <c r="H37" s="15">
+        <v>10</v>
+      </c>
+      <c r="I37" s="15">
+        <v>10</v>
+      </c>
+      <c r="J37" s="31">
+        <v>5</v>
+      </c>
+      <c r="K37" s="14">
+        <v>4</v>
+      </c>
+      <c r="L37" s="15">
+        <v>2</v>
+      </c>
+      <c r="M37" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="N37" s="31">
+        <v>4</v>
+      </c>
+      <c r="O37" s="14">
+        <v>12</v>
+      </c>
+      <c r="P37" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q37" s="15">
+        <v>50</v>
+      </c>
+      <c r="R37" s="31">
+        <v>5</v>
+      </c>
+      <c r="S37" s="14">
+        <v>12</v>
+      </c>
+      <c r="T37" s="15">
+        <v>10</v>
+      </c>
+      <c r="U37" s="15">
+        <v>10</v>
+      </c>
+      <c r="V37" s="31">
+        <v>5</v>
+      </c>
+      <c r="W37" s="14">
+        <v>12</v>
+      </c>
+      <c r="X37" s="15">
+        <v>2</v>
+      </c>
+      <c r="Y37" s="15">
+        <v>50</v>
+      </c>
+      <c r="Z37" s="31">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="38" ht="15" spans="2:26">
+      <c r="B38" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="20">
+        <v>4</v>
+      </c>
+      <c r="D38" s="21">
+        <v>10</v>
+      </c>
+      <c r="E38" s="21">
+        <v>10</v>
+      </c>
+      <c r="F38" s="33">
+        <v>4</v>
+      </c>
+      <c r="G38" s="20">
+        <v>12</v>
+      </c>
+      <c r="H38" s="21">
+        <v>10</v>
+      </c>
+      <c r="I38" s="21">
+        <v>1</v>
+      </c>
+      <c r="J38" s="33">
+        <v>5</v>
+      </c>
+      <c r="K38" s="20">
+        <v>4</v>
+      </c>
+      <c r="L38" s="21">
+        <v>10</v>
+      </c>
+      <c r="M38" s="21">
+        <v>1</v>
+      </c>
+      <c r="N38" s="33">
+        <v>4</v>
+      </c>
+      <c r="O38" s="20">
+        <v>4</v>
+      </c>
+      <c r="P38" s="21">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="21">
+        <v>10</v>
+      </c>
+      <c r="R38" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="S38" s="20">
+        <v>12</v>
+      </c>
+      <c r="T38" s="21">
+        <v>10</v>
+      </c>
+      <c r="U38" s="21">
+        <v>5</v>
+      </c>
+      <c r="V38" s="33">
+        <v>5</v>
+      </c>
+      <c r="W38" s="20">
+        <v>12</v>
+      </c>
+      <c r="X38" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y38" s="21">
+        <v>5</v>
+      </c>
+      <c r="Z38" s="33">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Figuras + txt tunings + txt execuções + Apresentações + ParamLivres
</commit_message>
<xml_diff>
--- a/Apresentacoes/PARAMETROSLIVRES_1.xlsx
+++ b/Apresentacoes/PARAMETROSLIVRES_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>GRIEWANGK</t>
   </si>
@@ -79,16 +79,64 @@
     <t>std | por</t>
   </si>
   <si>
-    <t>GEOreal2_P_VO_UNI</t>
-  </si>
-  <si>
-    <t>GEOreal2_N_VO_UNI</t>
-  </si>
-  <si>
-    <t>GEOreal2_P_DS_UNI</t>
-  </si>
-  <si>
-    <t>GEOreal2_N_DS_UNI</t>
+    <t>1 | 2</t>
+  </si>
+  <si>
+    <t>1 | 50</t>
+  </si>
+  <si>
+    <t>2 | 1</t>
+  </si>
+  <si>
+    <t>10 | 50</t>
+  </si>
+  <si>
+    <t>0,1 | 1</t>
+  </si>
+  <si>
+    <t>12 | 4</t>
+  </si>
+  <si>
+    <t>50 | 10</t>
+  </si>
+  <si>
+    <t>0,5 | 1</t>
+  </si>
+  <si>
+    <t>2 | 10</t>
+  </si>
+  <si>
+    <t>10 | 1</t>
+  </si>
+  <si>
+    <t>10 | 2</t>
+  </si>
+  <si>
+    <t>4 | 8</t>
+  </si>
+  <si>
+    <t>5 | 10</t>
+  </si>
+  <si>
+    <t>8 | 4</t>
+  </si>
+  <si>
+    <t>1 | 5</t>
+  </si>
+  <si>
+    <t>4 | 12</t>
+  </si>
+  <si>
+    <t>10 | 5</t>
+  </si>
+  <si>
+    <t>12 | 8</t>
+  </si>
+  <si>
+    <t>16 | 4</t>
+  </si>
+  <si>
+    <t>1 | 5 | 10</t>
   </si>
 </sst>
 </file>
@@ -96,12 +144,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,9 +166,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,15 +201,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,8 +217,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,9 +241,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,74 +317,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,199 +332,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,17 +686,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,6 +715,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,21 +775,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -733,152 +788,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -930,28 +985,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -975,16 +1045,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -992,6 +1068,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1312,16 +1391,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:AA38"/>
+  <dimension ref="B1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31:J31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38:O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.75" customWidth="1"/>
     <col min="2" max="2" width="21.125" customWidth="1"/>
+    <col min="13" max="14" width="12.625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15"/>
@@ -1331,37 +1411,37 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="25"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="25"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="25"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="25"/>
+      <c r="R2" s="30"/>
       <c r="S2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="25"/>
+      <c r="V2" s="30"/>
       <c r="W2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="25"/>
+      <c r="Z2" s="30"/>
     </row>
     <row r="3" ht="15" spans="3:26">
       <c r="C3" s="3" t="s">
@@ -1373,7 +1453,7 @@
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1385,7 +1465,7 @@
       <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -1397,7 +1477,7 @@
       <c r="M3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="N3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -1409,7 +1489,7 @@
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="S3" s="3" t="s">
@@ -1421,7 +1501,7 @@
       <c r="U3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="V3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="W3" s="3" t="s">
@@ -1433,7 +1513,7 @@
       <c r="Y3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="26" t="s">
+      <c r="Z3" s="31" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1445,42 +1525,42 @@
       <c r="E4">
         <v>0.8</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="32">
         <v>1.5</v>
       </c>
       <c r="G4" s="6"/>
       <c r="I4">
         <v>1.2</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="32">
         <v>1.5</v>
       </c>
       <c r="K4" s="6"/>
       <c r="M4">
         <v>2.4</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="32">
         <v>6.5</v>
       </c>
       <c r="O4" s="6"/>
       <c r="Q4">
         <v>0.6</v>
       </c>
-      <c r="R4" s="27">
+      <c r="R4" s="32">
         <v>8</v>
       </c>
       <c r="S4" s="6"/>
       <c r="U4">
         <v>0.8</v>
       </c>
-      <c r="V4" s="27">
+      <c r="V4" s="32">
         <v>1</v>
       </c>
       <c r="W4" s="6"/>
       <c r="Y4">
         <v>2</v>
       </c>
-      <c r="Z4" s="27">
+      <c r="Z4" s="32">
         <v>6</v>
       </c>
     </row>
@@ -1492,42 +1572,42 @@
       <c r="E5">
         <v>0.5</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="32">
         <v>4.5</v>
       </c>
       <c r="G5" s="6"/>
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="32">
         <v>5</v>
       </c>
       <c r="K5" s="6"/>
       <c r="M5">
         <v>0.5</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="32">
         <v>4.5</v>
       </c>
       <c r="O5" s="6"/>
       <c r="Q5">
         <v>7.5</v>
       </c>
-      <c r="R5" s="27">
+      <c r="R5" s="32">
         <v>3</v>
       </c>
       <c r="S5" s="6"/>
       <c r="U5">
         <v>1</v>
       </c>
-      <c r="V5" s="27">
+      <c r="V5" s="32">
         <v>5</v>
       </c>
       <c r="W5" s="6"/>
       <c r="Y5">
         <v>3</v>
       </c>
-      <c r="Z5" s="27">
+      <c r="Z5" s="32">
         <v>4</v>
       </c>
     </row>
@@ -1539,42 +1619,42 @@
       <c r="E6">
         <v>1.8</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="32">
         <v>1.5</v>
       </c>
       <c r="G6" s="6"/>
       <c r="I6">
         <v>0.4</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="32">
         <v>6</v>
       </c>
       <c r="K6" s="6"/>
       <c r="M6">
         <v>0.2</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="32">
         <v>5.5</v>
       </c>
       <c r="O6" s="6"/>
       <c r="Q6">
         <v>1.8</v>
       </c>
-      <c r="R6" s="27">
+      <c r="R6" s="32">
         <v>2</v>
       </c>
       <c r="S6" s="6"/>
       <c r="U6">
         <v>0.4</v>
       </c>
-      <c r="V6" s="27">
+      <c r="V6" s="32">
         <v>6.5</v>
       </c>
       <c r="W6" s="6"/>
       <c r="Y6">
         <v>0.2</v>
       </c>
-      <c r="Z6" s="27">
+      <c r="Z6" s="32">
         <v>2</v>
       </c>
     </row>
@@ -1591,7 +1671,7 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="32">
         <v>3</v>
       </c>
       <c r="G7" s="6">
@@ -1603,7 +1683,7 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="32">
         <v>5</v>
       </c>
       <c r="K7" s="6">
@@ -1615,7 +1695,7 @@
       <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="32">
         <v>5</v>
       </c>
       <c r="O7" s="6">
@@ -1627,7 +1707,7 @@
       <c r="Q7">
         <v>4</v>
       </c>
-      <c r="R7" s="27">
+      <c r="R7" s="32">
         <v>5</v>
       </c>
       <c r="S7" s="6">
@@ -1639,7 +1719,7 @@
       <c r="U7">
         <v>1</v>
       </c>
-      <c r="V7" s="27">
+      <c r="V7" s="32">
         <v>5</v>
       </c>
       <c r="W7" s="6">
@@ -1651,7 +1731,7 @@
       <c r="Y7">
         <v>1</v>
       </c>
-      <c r="Z7" s="27">
+      <c r="Z7" s="32">
         <v>3.5</v>
       </c>
     </row>
@@ -1668,7 +1748,7 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="32">
         <v>2.5</v>
       </c>
       <c r="G8" s="6">
@@ -1680,7 +1760,7 @@
       <c r="I8">
         <v>10</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="32">
         <v>5</v>
       </c>
       <c r="K8" s="6">
@@ -1692,7 +1772,7 @@
       <c r="M8">
         <v>0.3</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="32">
         <v>5</v>
       </c>
       <c r="O8" s="6">
@@ -1704,7 +1784,7 @@
       <c r="Q8">
         <v>10</v>
       </c>
-      <c r="R8" s="27">
+      <c r="R8" s="32">
         <v>3</v>
       </c>
       <c r="S8" s="6">
@@ -1716,7 +1796,7 @@
       <c r="U8">
         <v>5</v>
       </c>
-      <c r="V8" s="27">
+      <c r="V8" s="32">
         <v>5</v>
       </c>
       <c r="W8" s="6">
@@ -1728,7 +1808,7 @@
       <c r="Y8">
         <v>10</v>
       </c>
-      <c r="Z8" s="27">
+      <c r="Z8" s="32">
         <v>4</v>
       </c>
     </row>
@@ -1745,7 +1825,7 @@
       <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="32">
         <v>3</v>
       </c>
       <c r="G9" s="6">
@@ -1757,7 +1837,7 @@
       <c r="I9">
         <v>4</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="32">
         <v>5</v>
       </c>
       <c r="K9" s="6">
@@ -1769,7 +1849,7 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="32">
         <v>4.5</v>
       </c>
       <c r="O9" s="6">
@@ -1781,7 +1861,7 @@
       <c r="Q9">
         <v>4</v>
       </c>
-      <c r="R9" s="27">
+      <c r="R9" s="32">
         <v>3</v>
       </c>
       <c r="S9" s="6">
@@ -1793,7 +1873,7 @@
       <c r="U9">
         <v>4</v>
       </c>
-      <c r="V9" s="27">
+      <c r="V9" s="32">
         <v>5</v>
       </c>
       <c r="W9" s="6">
@@ -1805,7 +1885,7 @@
       <c r="Y9">
         <v>2</v>
       </c>
-      <c r="Z9" s="27">
+      <c r="Z9" s="32">
         <v>3.5</v>
       </c>
     </row>
@@ -1822,7 +1902,7 @@
       <c r="E10">
         <v>5</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="32">
         <v>4</v>
       </c>
       <c r="G10" s="6">
@@ -1834,7 +1914,7 @@
       <c r="I10">
         <v>5</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="32">
         <v>4.5</v>
       </c>
       <c r="K10" s="6">
@@ -1846,7 +1926,7 @@
       <c r="M10">
         <v>5</v>
       </c>
-      <c r="N10" s="27">
+      <c r="N10" s="32">
         <v>4</v>
       </c>
       <c r="O10" s="6">
@@ -1858,7 +1938,7 @@
       <c r="Q10">
         <v>5</v>
       </c>
-      <c r="R10" s="27">
+      <c r="R10" s="32">
         <v>5</v>
       </c>
       <c r="S10" s="6">
@@ -1870,7 +1950,7 @@
       <c r="U10">
         <v>1</v>
       </c>
-      <c r="V10" s="27">
+      <c r="V10" s="32">
         <v>5</v>
       </c>
       <c r="W10" s="6">
@@ -1882,7 +1962,7 @@
       <c r="Y10">
         <v>1</v>
       </c>
-      <c r="Z10" s="27">
+      <c r="Z10" s="32">
         <v>3</v>
       </c>
     </row>
@@ -1899,7 +1979,7 @@
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="32">
         <v>2.5</v>
       </c>
       <c r="G11" s="6">
@@ -1911,7 +1991,7 @@
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="32">
         <v>5</v>
       </c>
       <c r="K11" s="6">
@@ -1923,7 +2003,7 @@
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="N11" s="27">
+      <c r="N11" s="32">
         <v>5</v>
       </c>
       <c r="O11" s="6">
@@ -1935,7 +2015,7 @@
       <c r="Q11">
         <v>50</v>
       </c>
-      <c r="R11" s="27">
+      <c r="R11" s="32">
         <v>4.5</v>
       </c>
       <c r="S11" s="6">
@@ -1947,7 +2027,7 @@
       <c r="U11">
         <v>10</v>
       </c>
-      <c r="V11" s="27">
+      <c r="V11" s="32">
         <v>5</v>
       </c>
       <c r="W11" s="6">
@@ -1959,7 +2039,7 @@
       <c r="Y11">
         <v>10</v>
       </c>
-      <c r="Z11" s="27">
+      <c r="Z11" s="32">
         <v>3.5</v>
       </c>
     </row>
@@ -1976,7 +2056,7 @@
       <c r="E12" s="10">
         <v>10</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="33">
         <v>4.5</v>
       </c>
       <c r="G12" s="9">
@@ -1988,7 +2068,7 @@
       <c r="I12" s="10">
         <v>10</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="33">
         <v>5</v>
       </c>
       <c r="K12" s="9">
@@ -2000,7 +2080,7 @@
       <c r="M12" s="10">
         <v>1</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="33">
         <v>4</v>
       </c>
       <c r="O12" s="9">
@@ -2012,7 +2092,7 @@
       <c r="Q12" s="10">
         <v>10</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12" s="33">
         <v>2</v>
       </c>
       <c r="S12" s="9">
@@ -2024,7 +2104,7 @@
       <c r="U12" s="10">
         <v>10</v>
       </c>
-      <c r="V12" s="28">
+      <c r="V12" s="33">
         <v>4.5</v>
       </c>
       <c r="W12" s="9">
@@ -2036,7 +2116,7 @@
       <c r="Y12" s="10">
         <v>10</v>
       </c>
-      <c r="Z12" s="28">
+      <c r="Z12" s="33">
         <v>3</v>
       </c>
     </row>
@@ -2045,29 +2125,29 @@
       <c r="D18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="36"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="43"/>
     </row>
     <row r="19" ht="15" spans="4:14">
       <c r="D19" s="12"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="37"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="44"/>
     </row>
     <row r="23" ht="15"/>
     <row r="24" ht="15" spans="3:26">
@@ -2076,37 +2156,37 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="25"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="25"/>
+      <c r="J24" s="30"/>
       <c r="K24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="25"/>
+      <c r="N24" s="30"/>
       <c r="O24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="25"/>
+      <c r="R24" s="30"/>
       <c r="S24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="25"/>
+      <c r="V24" s="30"/>
       <c r="W24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-      <c r="Z24" s="25"/>
+      <c r="Z24" s="30"/>
     </row>
     <row r="25" ht="15" spans="3:26">
       <c r="C25" s="3" t="s">
@@ -2118,7 +2198,7 @@
       <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -2130,7 +2210,7 @@
       <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -2142,7 +2222,7 @@
       <c r="M25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N25" s="26" t="s">
+      <c r="N25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -2154,7 +2234,7 @@
       <c r="Q25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R25" s="26" t="s">
+      <c r="R25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -2166,7 +2246,7 @@
       <c r="U25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V25" s="26" t="s">
+      <c r="V25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="W25" s="3" t="s">
@@ -2178,7 +2258,7 @@
       <c r="Y25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Z25" s="26" t="s">
+      <c r="Z25" s="31" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2191,7 +2271,7 @@
       <c r="E26" s="15">
         <v>1</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="36">
         <v>1.5</v>
       </c>
       <c r="G26" s="14"/>
@@ -2199,7 +2279,7 @@
       <c r="I26" s="15">
         <v>1.8</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="36">
         <v>2</v>
       </c>
       <c r="K26" s="14"/>
@@ -2207,7 +2287,7 @@
       <c r="M26" s="15">
         <v>2.2</v>
       </c>
-      <c r="N26" s="31">
+      <c r="N26" s="36">
         <v>6</v>
       </c>
       <c r="O26" s="14"/>
@@ -2215,7 +2295,7 @@
       <c r="Q26" s="15">
         <v>1.8</v>
       </c>
-      <c r="R26" s="31">
+      <c r="R26" s="36">
         <v>6</v>
       </c>
       <c r="S26" s="14"/>
@@ -2223,7 +2303,7 @@
       <c r="U26" s="15">
         <v>0.8</v>
       </c>
-      <c r="V26" s="31">
+      <c r="V26" s="36">
         <v>1</v>
       </c>
       <c r="W26" s="14"/>
@@ -2231,7 +2311,7 @@
       <c r="Y26" s="15">
         <v>2</v>
       </c>
-      <c r="Z26" s="31">
+      <c r="Z26" s="36">
         <v>5</v>
       </c>
       <c r="AA26" s="15"/>
@@ -2245,7 +2325,7 @@
       <c r="E27" s="15">
         <v>0.5</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="36">
         <v>6</v>
       </c>
       <c r="G27" s="14"/>
@@ -2253,7 +2333,7 @@
       <c r="I27" s="15">
         <v>3</v>
       </c>
-      <c r="J27" s="31">
+      <c r="J27" s="36">
         <v>5</v>
       </c>
       <c r="K27" s="14"/>
@@ -2261,7 +2341,7 @@
       <c r="M27" s="15">
         <v>0.5</v>
       </c>
-      <c r="N27" s="31">
+      <c r="N27" s="36">
         <v>6</v>
       </c>
       <c r="O27" s="14"/>
@@ -2269,7 +2349,7 @@
       <c r="Q27" s="15">
         <v>8</v>
       </c>
-      <c r="R27" s="31">
+      <c r="R27" s="36">
         <v>2.5</v>
       </c>
       <c r="S27" s="14"/>
@@ -2277,7 +2357,7 @@
       <c r="U27" s="15">
         <v>1</v>
       </c>
-      <c r="V27" s="31">
+      <c r="V27" s="36">
         <v>5</v>
       </c>
       <c r="W27" s="14"/>
@@ -2285,7 +2365,7 @@
       <c r="Y27" s="15">
         <v>1.5</v>
       </c>
-      <c r="Z27" s="31">
+      <c r="Z27" s="36">
         <v>1.5</v>
       </c>
       <c r="AA27" s="15"/>
@@ -2299,7 +2379,7 @@
       <c r="E28" s="15">
         <v>2</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="36">
         <v>1.5</v>
       </c>
       <c r="G28" s="14"/>
@@ -2307,7 +2387,7 @@
       <c r="I28" s="15">
         <v>0.4</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="36">
         <v>6</v>
       </c>
       <c r="K28" s="14"/>
@@ -2315,7 +2395,7 @@
       <c r="M28" s="15">
         <v>0.2</v>
       </c>
-      <c r="N28" s="31">
+      <c r="N28" s="36">
         <v>5</v>
       </c>
       <c r="O28" s="14"/>
@@ -2323,7 +2403,7 @@
       <c r="Q28" s="15">
         <v>1.4</v>
       </c>
-      <c r="R28" s="31">
+      <c r="R28" s="36">
         <v>1.5</v>
       </c>
       <c r="S28" s="14"/>
@@ -2331,7 +2411,7 @@
       <c r="U28" s="15">
         <v>0.6</v>
       </c>
-      <c r="V28" s="31">
+      <c r="V28" s="36">
         <v>6</v>
       </c>
       <c r="W28" s="14"/>
@@ -2339,163 +2419,163 @@
       <c r="Y28" s="15">
         <v>0.2</v>
       </c>
-      <c r="Z28" s="31">
+      <c r="Z28" s="36">
         <v>2</v>
       </c>
       <c r="AA28" s="15"/>
     </row>
     <row r="29" spans="2:27">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="14">
-        <v>4</v>
-      </c>
-      <c r="D29" s="15">
-        <v>1</v>
-      </c>
-      <c r="E29" s="15">
-        <v>1</v>
-      </c>
-      <c r="F29" s="31">
+      <c r="C29" s="18">
+        <v>4</v>
+      </c>
+      <c r="D29" s="19">
+        <v>1</v>
+      </c>
+      <c r="E29" s="19">
+        <v>1</v>
+      </c>
+      <c r="F29" s="37">
         <v>2.5</v>
       </c>
-      <c r="G29" s="14">
-        <v>4</v>
-      </c>
-      <c r="H29" s="15">
-        <v>1</v>
-      </c>
-      <c r="I29" s="15">
-        <v>1</v>
-      </c>
-      <c r="J29" s="31">
+      <c r="G29" s="18">
+        <v>4</v>
+      </c>
+      <c r="H29" s="19">
+        <v>1</v>
+      </c>
+      <c r="I29" s="19">
+        <v>1</v>
+      </c>
+      <c r="J29" s="37">
         <v>4.5</v>
       </c>
-      <c r="K29" s="14">
-        <v>4</v>
-      </c>
-      <c r="L29" s="15">
-        <v>2</v>
-      </c>
-      <c r="M29" s="15">
-        <v>1</v>
-      </c>
-      <c r="N29" s="31">
-        <v>5</v>
-      </c>
-      <c r="O29" s="14">
+      <c r="K29" s="18">
+        <v>4</v>
+      </c>
+      <c r="L29" s="19">
+        <v>2</v>
+      </c>
+      <c r="M29" s="19">
+        <v>1</v>
+      </c>
+      <c r="N29" s="37">
+        <v>5</v>
+      </c>
+      <c r="O29" s="18">
         <v>16</v>
       </c>
-      <c r="P29" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q29" s="15">
+      <c r="P29" s="19">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="19">
         <v>8</v>
       </c>
-      <c r="R29" s="31">
-        <v>4</v>
-      </c>
-      <c r="S29" s="14">
-        <v>4</v>
-      </c>
-      <c r="T29" s="15">
-        <v>1</v>
-      </c>
-      <c r="U29" s="15">
-        <v>1</v>
-      </c>
-      <c r="V29" s="31">
-        <v>5</v>
-      </c>
-      <c r="W29" s="14">
+      <c r="R29" s="37">
+        <v>4</v>
+      </c>
+      <c r="S29" s="18">
+        <v>4</v>
+      </c>
+      <c r="T29" s="19">
+        <v>1</v>
+      </c>
+      <c r="U29" s="19">
+        <v>1</v>
+      </c>
+      <c r="V29" s="37">
+        <v>5</v>
+      </c>
+      <c r="W29" s="18">
         <v>8</v>
       </c>
-      <c r="X29" s="15">
-        <v>2</v>
-      </c>
-      <c r="Y29" s="15">
-        <v>2</v>
-      </c>
-      <c r="Z29" s="31">
+      <c r="X29" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y29" s="19">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="37">
         <v>4</v>
       </c>
       <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="2:27">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="21">
         <v>12</v>
       </c>
-      <c r="D30" s="18">
-        <v>1</v>
-      </c>
-      <c r="E30" s="18">
-        <v>1</v>
-      </c>
-      <c r="F30" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="G30" s="32">
+      <c r="D30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="21">
+        <v>3</v>
+      </c>
+      <c r="G30" s="22">
         <v>12</v>
       </c>
-      <c r="H30" s="18">
-        <v>2</v>
-      </c>
-      <c r="I30" s="18">
-        <v>10</v>
-      </c>
-      <c r="J30" s="35">
-        <v>5</v>
-      </c>
-      <c r="K30" s="32">
-        <v>4</v>
-      </c>
-      <c r="L30" s="18">
-        <v>1</v>
-      </c>
-      <c r="M30" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="N30" s="35">
-        <v>4</v>
-      </c>
-      <c r="O30" s="32">
+      <c r="H30" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="38">
+        <v>5</v>
+      </c>
+      <c r="K30" s="22">
+        <v>4</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="38">
+        <v>4</v>
+      </c>
+      <c r="O30" s="22">
         <v>12</v>
       </c>
-      <c r="P30" s="18">
-        <v>2</v>
-      </c>
-      <c r="Q30" s="18">
+      <c r="P30" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q30" s="21">
         <v>50</v>
       </c>
-      <c r="R30" s="35">
-        <v>5</v>
-      </c>
-      <c r="S30" s="32">
+      <c r="R30" s="38">
+        <v>4.5</v>
+      </c>
+      <c r="S30" s="22">
         <v>12</v>
       </c>
-      <c r="T30" s="18">
-        <v>2</v>
-      </c>
-      <c r="U30" s="18">
-        <v>10</v>
-      </c>
-      <c r="V30" s="35">
-        <v>5</v>
-      </c>
-      <c r="W30" s="32">
-        <v>12</v>
-      </c>
-      <c r="X30" s="18">
-        <v>1</v>
-      </c>
-      <c r="Y30" s="18">
-        <v>50</v>
-      </c>
-      <c r="Z30" s="35">
+      <c r="T30" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="U30" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="V30" s="38">
+        <v>4.5</v>
+      </c>
+      <c r="W30" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="X30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y30" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z30" s="38">
         <v>3.5</v>
       </c>
       <c r="AA30" s="15"/>
@@ -2504,154 +2584,154 @@
       <c r="B31" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="14">
-        <v>4</v>
-      </c>
-      <c r="D31" s="15">
-        <v>2</v>
-      </c>
-      <c r="E31" s="15">
-        <v>2</v>
-      </c>
-      <c r="F31" s="31">
-        <v>2.5</v>
-      </c>
-      <c r="G31" s="14">
+      <c r="C31" s="22">
+        <v>4</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="21">
+        <v>2</v>
+      </c>
+      <c r="F31" s="38">
+        <v>3</v>
+      </c>
+      <c r="G31" s="22">
         <v>12</v>
       </c>
-      <c r="H31" s="15">
-        <v>2</v>
-      </c>
-      <c r="I31" s="15">
-        <v>1</v>
-      </c>
-      <c r="J31" s="31">
-        <v>5</v>
-      </c>
-      <c r="K31" s="14">
-        <v>4</v>
-      </c>
-      <c r="L31" s="15">
-        <v>2</v>
-      </c>
-      <c r="M31" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="N31" s="31">
-        <v>5</v>
-      </c>
-      <c r="O31" s="14">
-        <v>4</v>
-      </c>
-      <c r="P31" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="15">
-        <v>2</v>
-      </c>
-      <c r="R31" s="31">
-        <v>4</v>
-      </c>
-      <c r="S31" s="14">
+      <c r="H31" s="21">
+        <v>2</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="38">
+        <v>5</v>
+      </c>
+      <c r="K31" s="22">
+        <v>4</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="N31" s="38">
+        <v>4.5</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="P31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="R31" s="38">
+        <v>4</v>
+      </c>
+      <c r="S31" s="22">
         <v>12</v>
       </c>
-      <c r="T31" s="15">
-        <v>2</v>
-      </c>
-      <c r="U31" s="15">
-        <v>2</v>
-      </c>
-      <c r="V31" s="31">
+      <c r="T31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="U31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="V31" s="38">
         <v>4.5</v>
       </c>
-      <c r="W31" s="14">
+      <c r="W31" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="X31" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z31" s="38">
+        <v>3</v>
+      </c>
+      <c r="AA31" s="15"/>
+    </row>
+    <row r="32" spans="2:27">
+      <c r="B32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="24">
+        <v>4</v>
+      </c>
+      <c r="D32" s="25">
+        <v>2</v>
+      </c>
+      <c r="E32" s="25">
+        <v>5</v>
+      </c>
+      <c r="F32" s="39">
+        <v>5</v>
+      </c>
+      <c r="G32" s="24">
+        <v>4</v>
+      </c>
+      <c r="H32" s="25">
+        <v>2</v>
+      </c>
+      <c r="I32" s="25">
+        <v>5</v>
+      </c>
+      <c r="J32" s="39">
+        <v>4.5</v>
+      </c>
+      <c r="K32" s="24">
         <v>12</v>
       </c>
-      <c r="X31" s="15">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="15">
-        <v>2</v>
-      </c>
-      <c r="Z31" s="31">
-        <v>2.5</v>
-      </c>
-      <c r="AA31" s="15"/>
-    </row>
-    <row r="32" spans="2:27">
-      <c r="B32" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="14">
-        <v>4</v>
-      </c>
-      <c r="D32" s="15">
-        <v>2</v>
-      </c>
-      <c r="E32" s="15">
-        <v>5</v>
-      </c>
-      <c r="F32" s="31">
-        <v>5</v>
-      </c>
-      <c r="G32" s="14">
-        <v>4</v>
-      </c>
-      <c r="H32" s="15">
-        <v>2</v>
-      </c>
-      <c r="I32" s="15">
-        <v>5</v>
-      </c>
-      <c r="J32" s="31">
-        <v>4.5</v>
-      </c>
-      <c r="K32" s="14">
+      <c r="L32" s="25">
+        <v>2</v>
+      </c>
+      <c r="M32" s="25">
+        <v>5</v>
+      </c>
+      <c r="N32" s="39">
+        <v>5</v>
+      </c>
+      <c r="O32" s="24">
         <v>12</v>
       </c>
-      <c r="L32" s="15">
-        <v>2</v>
-      </c>
-      <c r="M32" s="15">
-        <v>5</v>
-      </c>
-      <c r="N32" s="31">
-        <v>5</v>
-      </c>
-      <c r="O32" s="14">
-        <v>12</v>
-      </c>
-      <c r="P32" s="15">
+      <c r="P32" s="25">
         <v>10</v>
       </c>
-      <c r="Q32" s="15">
-        <v>5</v>
-      </c>
-      <c r="R32" s="31">
-        <v>5</v>
-      </c>
-      <c r="S32" s="14">
-        <v>4</v>
-      </c>
-      <c r="T32" s="15">
-        <v>2</v>
-      </c>
-      <c r="U32" s="15">
-        <v>1</v>
-      </c>
-      <c r="V32" s="31">
-        <v>5</v>
-      </c>
-      <c r="W32" s="14">
-        <v>4</v>
-      </c>
-      <c r="X32" s="15">
+      <c r="Q32" s="25">
+        <v>5</v>
+      </c>
+      <c r="R32" s="39">
+        <v>5</v>
+      </c>
+      <c r="S32" s="24">
+        <v>4</v>
+      </c>
+      <c r="T32" s="25">
+        <v>2</v>
+      </c>
+      <c r="U32" s="25">
+        <v>1</v>
+      </c>
+      <c r="V32" s="39">
+        <v>5</v>
+      </c>
+      <c r="W32" s="24">
+        <v>4</v>
+      </c>
+      <c r="X32" s="25">
         <v>10</v>
       </c>
-      <c r="Y32" s="15">
-        <v>1</v>
-      </c>
-      <c r="Z32" s="31">
+      <c r="Y32" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="39">
         <v>5</v>
       </c>
       <c r="AA32" s="15"/>
@@ -2660,465 +2740,190 @@
       <c r="B33" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="38">
+        <v>3</v>
+      </c>
+      <c r="G33" s="22">
         <v>12</v>
       </c>
-      <c r="D33" s="15">
-        <v>2</v>
-      </c>
-      <c r="E33" s="15">
-        <v>5</v>
-      </c>
-      <c r="F33" s="31">
+      <c r="H33" s="21">
+        <v>10</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="38">
+        <v>5</v>
+      </c>
+      <c r="K33" s="22">
+        <v>4</v>
+      </c>
+      <c r="L33" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" s="38">
+        <v>4</v>
+      </c>
+      <c r="O33" s="22">
+        <v>12</v>
+      </c>
+      <c r="P33" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>50</v>
+      </c>
+      <c r="R33" s="38">
+        <v>4</v>
+      </c>
+      <c r="S33" s="22">
+        <v>12</v>
+      </c>
+      <c r="T33" s="21">
+        <v>10</v>
+      </c>
+      <c r="U33" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="V33" s="38">
+        <v>5</v>
+      </c>
+      <c r="W33" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="X33" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y33" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z33" s="38">
+        <v>3.5</v>
+      </c>
+      <c r="AA33" s="15"/>
+    </row>
+    <row r="34" ht="15" spans="2:27">
+      <c r="B34" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="41">
         <v>3</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G34" s="42">
         <v>12</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H34" s="40">
         <v>10</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I34" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34" s="41">
+        <v>5</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L34" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" s="41">
+        <v>4</v>
+      </c>
+      <c r="O34" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q34" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="R34" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="S34" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="T34" s="40">
         <v>10</v>
       </c>
-      <c r="J33" s="31">
+      <c r="U34" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="V34" s="41">
         <v>4.5</v>
       </c>
-      <c r="K33" s="14">
-        <v>4</v>
-      </c>
-      <c r="L33" s="15">
-        <v>2</v>
-      </c>
-      <c r="M33" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="N33" s="31">
-        <v>5</v>
-      </c>
-      <c r="O33" s="14">
-        <v>12</v>
-      </c>
-      <c r="P33" s="15">
-        <v>10</v>
-      </c>
-      <c r="Q33" s="15">
-        <v>50</v>
-      </c>
-      <c r="R33" s="31">
-        <v>4.5</v>
-      </c>
-      <c r="S33" s="14">
-        <v>12</v>
-      </c>
-      <c r="T33" s="15">
-        <v>10</v>
-      </c>
-      <c r="U33" s="15">
-        <v>5</v>
-      </c>
-      <c r="V33" s="31">
-        <v>5</v>
-      </c>
-      <c r="W33" s="14">
-        <v>12</v>
-      </c>
-      <c r="X33" s="15">
-        <v>2</v>
-      </c>
-      <c r="Y33" s="15">
-        <v>50</v>
-      </c>
-      <c r="Z33" s="31">
+      <c r="W34" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="X34" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y34" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z34" s="41">
         <v>3</v>
       </c>
-      <c r="AA33" s="15"/>
-    </row>
-    <row r="34" ht="15" spans="2:27">
-      <c r="B34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="20">
-        <v>4</v>
-      </c>
-      <c r="D34" s="21">
-        <v>10</v>
-      </c>
-      <c r="E34" s="21">
-        <v>5</v>
-      </c>
-      <c r="F34" s="33">
-        <v>4</v>
-      </c>
-      <c r="G34" s="20">
-        <v>16</v>
-      </c>
-      <c r="H34" s="21">
-        <v>10</v>
-      </c>
-      <c r="I34" s="21">
-        <v>10</v>
-      </c>
-      <c r="J34" s="33">
-        <v>5</v>
-      </c>
-      <c r="K34" s="20">
-        <v>8</v>
-      </c>
-      <c r="L34" s="21">
-        <v>2</v>
-      </c>
-      <c r="M34" s="21">
-        <v>1</v>
-      </c>
-      <c r="N34" s="33">
-        <v>5</v>
-      </c>
-      <c r="O34" s="20">
-        <v>4</v>
-      </c>
-      <c r="P34" s="21">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="21">
-        <v>10</v>
-      </c>
-      <c r="R34" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="S34" s="20">
-        <v>16</v>
-      </c>
-      <c r="T34" s="21">
-        <v>10</v>
-      </c>
-      <c r="U34" s="21">
-        <v>5</v>
-      </c>
-      <c r="V34" s="33">
-        <v>5</v>
-      </c>
-      <c r="W34" s="20">
-        <v>16</v>
-      </c>
-      <c r="X34" s="21">
-        <v>2</v>
-      </c>
-      <c r="Y34" s="21">
-        <v>5</v>
-      </c>
-      <c r="Z34" s="33">
-        <v>2.5</v>
-      </c>
       <c r="AA34" s="15"/>
     </row>
-    <row r="35" spans="2:26">
-      <c r="B35" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="23">
-        <v>12</v>
-      </c>
-      <c r="D35" s="24">
-        <v>1</v>
-      </c>
-      <c r="E35" s="24">
-        <v>1</v>
-      </c>
-      <c r="F35" s="34">
-        <v>2.5</v>
-      </c>
-      <c r="G35" s="23">
-        <v>12</v>
-      </c>
-      <c r="H35" s="24">
-        <v>2</v>
-      </c>
-      <c r="I35" s="24">
-        <v>10</v>
-      </c>
-      <c r="J35" s="34">
-        <v>5</v>
-      </c>
-      <c r="K35" s="23">
-        <v>4</v>
-      </c>
-      <c r="L35" s="24">
-        <v>1</v>
-      </c>
-      <c r="M35" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="N35" s="34">
-        <v>4</v>
-      </c>
-      <c r="O35" s="23">
-        <v>12</v>
-      </c>
-      <c r="P35" s="24">
-        <v>2</v>
-      </c>
-      <c r="Q35" s="24">
-        <v>50</v>
-      </c>
-      <c r="R35" s="34">
-        <v>5</v>
-      </c>
-      <c r="S35" s="23">
-        <v>12</v>
-      </c>
-      <c r="T35" s="24">
-        <v>2</v>
-      </c>
-      <c r="U35" s="24">
-        <v>10</v>
-      </c>
-      <c r="V35" s="34">
-        <v>5</v>
-      </c>
-      <c r="W35" s="23">
-        <v>12</v>
-      </c>
-      <c r="X35" s="24">
-        <v>1</v>
-      </c>
-      <c r="Y35" s="24">
-        <v>50</v>
-      </c>
-      <c r="Z35" s="34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:26">
-      <c r="B36" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="14">
-        <v>4</v>
-      </c>
-      <c r="D36" s="15">
-        <v>2</v>
-      </c>
-      <c r="E36" s="15">
-        <v>2</v>
-      </c>
-      <c r="F36" s="31">
-        <v>2.5</v>
-      </c>
-      <c r="G36" s="14">
-        <v>12</v>
-      </c>
-      <c r="H36" s="15">
-        <v>2</v>
-      </c>
-      <c r="I36" s="15">
-        <v>2</v>
-      </c>
-      <c r="J36" s="31">
-        <v>5</v>
-      </c>
-      <c r="K36" s="14">
-        <v>4</v>
-      </c>
-      <c r="L36" s="15">
-        <v>2</v>
-      </c>
-      <c r="M36" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="N36" s="31">
-        <v>5</v>
-      </c>
-      <c r="O36" s="14">
-        <v>12</v>
-      </c>
-      <c r="P36" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q36" s="15">
-        <v>2</v>
-      </c>
-      <c r="R36" s="31">
-        <v>4</v>
-      </c>
-      <c r="S36" s="14">
-        <v>12</v>
-      </c>
-      <c r="T36" s="15">
-        <v>2</v>
-      </c>
-      <c r="U36" s="15">
-        <v>2</v>
-      </c>
-      <c r="V36" s="31">
-        <v>5</v>
-      </c>
-      <c r="W36" s="14">
-        <v>12</v>
-      </c>
-      <c r="X36" s="15">
-        <v>1</v>
-      </c>
-      <c r="Y36" s="15">
-        <v>2</v>
-      </c>
-      <c r="Z36" s="31">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:26">
-      <c r="B37" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="14">
-        <v>4</v>
-      </c>
-      <c r="D37" s="15">
-        <v>10</v>
-      </c>
-      <c r="E37" s="15">
-        <v>1</v>
-      </c>
-      <c r="F37" s="31">
-        <v>4</v>
-      </c>
-      <c r="G37" s="14">
-        <v>12</v>
-      </c>
-      <c r="H37" s="15">
-        <v>10</v>
-      </c>
-      <c r="I37" s="15">
-        <v>10</v>
-      </c>
-      <c r="J37" s="31">
-        <v>5</v>
-      </c>
-      <c r="K37" s="14">
-        <v>4</v>
-      </c>
-      <c r="L37" s="15">
-        <v>2</v>
-      </c>
-      <c r="M37" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="N37" s="31">
-        <v>4</v>
-      </c>
-      <c r="O37" s="14">
-        <v>12</v>
-      </c>
-      <c r="P37" s="15">
-        <v>10</v>
-      </c>
-      <c r="Q37" s="15">
-        <v>50</v>
-      </c>
-      <c r="R37" s="31">
-        <v>5</v>
-      </c>
-      <c r="S37" s="14">
-        <v>12</v>
-      </c>
-      <c r="T37" s="15">
-        <v>10</v>
-      </c>
-      <c r="U37" s="15">
-        <v>10</v>
-      </c>
-      <c r="V37" s="31">
-        <v>5</v>
-      </c>
-      <c r="W37" s="14">
-        <v>12</v>
-      </c>
-      <c r="X37" s="15">
-        <v>2</v>
-      </c>
-      <c r="Y37" s="15">
-        <v>50</v>
-      </c>
-      <c r="Z37" s="31">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="38" ht="15" spans="2:26">
-      <c r="B38" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="20">
-        <v>4</v>
-      </c>
-      <c r="D38" s="21">
-        <v>10</v>
-      </c>
-      <c r="E38" s="21">
-        <v>10</v>
-      </c>
-      <c r="F38" s="33">
-        <v>4</v>
-      </c>
-      <c r="G38" s="20">
-        <v>12</v>
-      </c>
-      <c r="H38" s="21">
-        <v>10</v>
-      </c>
-      <c r="I38" s="21">
-        <v>1</v>
-      </c>
-      <c r="J38" s="33">
-        <v>5</v>
-      </c>
-      <c r="K38" s="20">
-        <v>4</v>
-      </c>
-      <c r="L38" s="21">
-        <v>10</v>
-      </c>
-      <c r="M38" s="21">
-        <v>1</v>
-      </c>
-      <c r="N38" s="33">
-        <v>4</v>
-      </c>
-      <c r="O38" s="20">
-        <v>4</v>
-      </c>
-      <c r="P38" s="21">
-        <v>2</v>
-      </c>
-      <c r="Q38" s="21">
-        <v>10</v>
-      </c>
-      <c r="R38" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="S38" s="20">
-        <v>12</v>
-      </c>
-      <c r="T38" s="21">
-        <v>10</v>
-      </c>
-      <c r="U38" s="21">
-        <v>5</v>
-      </c>
-      <c r="V38" s="33">
-        <v>5</v>
-      </c>
-      <c r="W38" s="20">
-        <v>12</v>
-      </c>
-      <c r="X38" s="21">
-        <v>2</v>
-      </c>
-      <c r="Y38" s="21">
-        <v>5</v>
-      </c>
-      <c r="Z38" s="33">
-        <v>3.5</v>
-      </c>
+    <row r="65" spans="13:13">
+      <c r="M65" s="45"/>
+    </row>
+    <row r="66" spans="13:13">
+      <c r="M66" s="45"/>
+    </row>
+    <row r="67" spans="13:13">
+      <c r="M67" s="45"/>
+    </row>
+    <row r="68" spans="13:13">
+      <c r="M68" s="45"/>
+    </row>
+    <row r="69" spans="13:13">
+      <c r="M69" s="45"/>
+    </row>
+    <row r="70" spans="13:13">
+      <c r="M70" s="45"/>
+    </row>
+    <row r="71" spans="13:13">
+      <c r="M71" s="45"/>
+    </row>
+    <row r="72" spans="13:13">
+      <c r="M72" s="45"/>
+    </row>
+    <row r="73" spans="13:13">
+      <c r="M73" s="45"/>
+    </row>
+    <row r="74" spans="13:13">
+      <c r="M74" s="45"/>
+    </row>
+    <row r="75" spans="13:13">
+      <c r="M75" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>